<commit_message>
ajustes en diseño de la pagina principal
</commit_message>
<xml_diff>
--- a/Backend/doc/PlantillaMovil.xlsx
+++ b/Backend/doc/PlantillaMovil.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36431706-CF49-4911-BF0D-4EB40D9C7C07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <si>
     <t xml:space="preserve">FORMATO  </t>
   </si>
@@ -157,18 +157,45 @@
   <si>
     <t>fgjhdskghkfjghsdukfds</t>
   </si>
+  <si>
+    <t xml:space="preserve">United States</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PPD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-12-13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dsadawd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gfdgdfghdh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$10,000.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$100,000.00</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts>
     <numFmt numFmtId="7" formatCode="&quot;$&quot;#,##0.00_);\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
     <numFmt numFmtId="165" formatCode="#,##0%"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -274,7 +301,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills>
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -307,7 +334,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders>
     <border>
       <left/>
       <right/>
@@ -474,7 +501,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -968,7 +995,6 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
@@ -998,7 +1024,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="58" t="s">
+      <c r="A1" t="s" s="58">
         <v>0</v>
       </c>
       <c r="B1" s="58"/>
@@ -1028,7 +1054,7 @@
       <c r="Z1" s="3"/>
     </row>
     <row r="2" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="59" t="s">
+      <c r="A2" t="s" s="59">
         <v>1</v>
       </c>
       <c r="B2" s="59"/>
@@ -1058,11 +1084,11 @@
       <c r="Z2" s="3"/>
     </row>
     <row r="3" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" t="s" s="6">
         <v>2</v>
       </c>
-      <c r="B3" s="56" t="s">
-        <v>36</v>
+      <c r="B3" t="s" s="56">
+        <v>41</v>
       </c>
       <c r="C3" s="57"/>
       <c r="D3" s="57"/>
@@ -1084,10 +1110,10 @@
       <c r="Z3" s="3"/>
     </row>
     <row r="4" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" t="s" s="6">
         <v>3</v>
       </c>
-      <c r="B4" s="56" t="s">
+      <c r="B4" t="s" s="56">
         <v>24</v>
       </c>
       <c r="C4" s="57"/>
@@ -1113,10 +1139,10 @@
       <c r="Z4" s="3"/>
     </row>
     <row r="5" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" t="s" s="6">
         <v>4</v>
       </c>
-      <c r="B5" s="56" t="s">
+      <c r="B5" t="s" s="56">
         <v>25</v>
       </c>
       <c r="C5" s="57"/>
@@ -1142,10 +1168,10 @@
       <c r="Z5" s="3"/>
     </row>
     <row r="6" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="A6" t="s" s="9">
         <v>5</v>
       </c>
-      <c r="B6" s="56" t="s">
+      <c r="B6" t="s" s="56">
         <v>26</v>
       </c>
       <c r="C6" s="57"/>
@@ -1171,11 +1197,11 @@
       <c r="Z6" s="3"/>
     </row>
     <row r="7" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" t="s" s="6">
         <v>6</v>
       </c>
-      <c r="B7" s="56" t="s">
-        <v>37</v>
+      <c r="B7" t="s" s="56">
+        <v>42</v>
       </c>
       <c r="C7" s="57"/>
       <c r="D7" s="57"/>
@@ -1225,10 +1251,10 @@
       <c r="Z8" s="3"/>
     </row>
     <row r="9" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" t="s" s="6">
         <v>7</v>
       </c>
-      <c r="B9" s="60" t="s">
+      <c r="B9" t="s" s="60">
         <v>27</v>
       </c>
       <c r="C9" s="60"/>
@@ -1251,11 +1277,11 @@
       <c r="Z9" s="5"/>
     </row>
     <row r="10" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" t="s" s="3">
         <v>8</v>
       </c>
-      <c r="B10" s="61" t="s">
-        <v>32</v>
+      <c r="B10" t="s" s="61">
+        <v>43</v>
       </c>
       <c r="C10" s="61"/>
       <c r="D10" s="61"/>
@@ -1277,11 +1303,11 @@
       <c r="Z10" s="3"/>
     </row>
     <row r="11" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="A11" t="s" s="6">
         <v>9</v>
       </c>
-      <c r="B11" s="60" t="s">
-        <v>38</v>
+      <c r="B11" t="s" s="60">
+        <v>44</v>
       </c>
       <c r="C11" s="60"/>
       <c r="D11" s="60"/>
@@ -1303,10 +1329,10 @@
       <c r="Z11" s="3"/>
     </row>
     <row r="12" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" t="s" s="6">
         <v>10</v>
       </c>
-      <c r="B12" s="60" t="s">
+      <c r="B12" t="s" s="60">
         <v>28</v>
       </c>
       <c r="C12" s="60"/>
@@ -1332,11 +1358,11 @@
       <c r="Z12" s="3"/>
     </row>
     <row r="13" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="A13" t="s" s="6">
         <v>11</v>
       </c>
-      <c r="B13" s="62" t="s">
-        <v>39</v>
+      <c r="B13" t="s" s="62">
+        <v>45</v>
       </c>
       <c r="C13" s="62"/>
       <c r="D13" s="62"/>
@@ -1361,11 +1387,11 @@
       <c r="Z13" s="3"/>
     </row>
     <row r="14" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+      <c r="A14" t="s" s="6">
         <v>12</v>
       </c>
-      <c r="B14" s="60" t="s">
-        <v>29</v>
+      <c r="B14" t="s" s="60">
+        <v>46</v>
       </c>
       <c r="C14" s="60"/>
       <c r="D14" s="60"/>
@@ -1413,13 +1439,13 @@
       <c r="Z15" s="3"/>
     </row>
     <row r="16" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="18" t="s">
+      <c r="A16" t="s" s="18">
         <v>13</v>
       </c>
-      <c r="B16" s="18" t="s">
+      <c r="B16" t="s" s="18">
         <v>14</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" t="s" s="18">
         <v>15</v>
       </c>
       <c r="D16" s="7"/>
@@ -1467,13 +1493,13 @@
       <c r="Z17" s="3"/>
     </row>
     <row r="18" spans="1:26" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="20" t="s">
+      <c r="A18" t="s" s="20">
         <v>33</v>
       </c>
-      <c r="B18" s="20" t="s">
+      <c r="B18" t="s" s="20">
         <v>30</v>
       </c>
-      <c r="C18" s="21" t="s">
+      <c r="C18" t="s" s="21">
         <v>34</v>
       </c>
       <c r="D18" s="7"/>
@@ -1582,7 +1608,7 @@
       <c r="Z21" s="3"/>
     </row>
     <row r="22" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="47" t="s">
+      <c r="A22" t="s" s="47">
         <v>16</v>
       </c>
       <c r="B22" s="48"/>
@@ -1632,8 +1658,8 @@
       <c r="Z23" s="3"/>
     </row>
     <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="50" t="s">
-        <v>40</v>
+      <c r="A24" t="s" s="50">
+        <v>47</v>
       </c>
       <c r="B24" s="51"/>
       <c r="C24" s="51"/>
@@ -1686,11 +1712,11 @@
       <c r="Z25" s="3"/>
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="53" t="s">
+      <c r="A26" t="s" s="53">
         <v>17</v>
       </c>
       <c r="B26" s="49"/>
-      <c r="C26" s="53" t="s">
+      <c r="C26" t="s" s="53">
         <v>18</v>
       </c>
       <c r="D26" s="49"/>
@@ -1746,12 +1772,12 @@
       <c r="Z27" s="3"/>
     </row>
     <row r="28" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="41">
-        <v>50000</v>
+      <c r="A28" t="s" s="41">
+        <v>48</v>
       </c>
       <c r="B28" s="42"/>
-      <c r="C28" s="43">
-        <v>100000</v>
+      <c r="C28" t="s" s="43">
+        <v>49</v>
       </c>
       <c r="D28" s="44"/>
       <c r="E28" s="6"/>
@@ -1834,22 +1860,21 @@
       <c r="Z30" s="3"/>
     </row>
     <row r="31" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="32" t="s">
+      <c r="A31" t="s" s="32">
         <v>19</v>
       </c>
-      <c r="B31" s="32" t="s">
+      <c r="B31" t="s" s="32">
         <v>20</v>
       </c>
       <c r="C31" s="32"/>
       <c r="D31" s="32"/>
       <c r="E31" s="33"/>
-      <c r="F31" s="34" t="s">
+      <c r="F31" t="s" s="34">
         <v>21</v>
       </c>
       <c r="G31" s="34"/>
       <c r="H31" s="36">
         <f>SUM(C28)</f>
-        <v>100000</v>
       </c>
       <c r="I31" s="37"/>
       <c r="J31" s="3"/>
@@ -1871,22 +1896,21 @@
       <c r="Z31" s="3"/>
     </row>
     <row r="32" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="35" t="s">
+      <c r="A32" t="s" s="35">
         <v>35</v>
       </c>
-      <c r="B32" s="38" t="s">
+      <c r="B32" t="s" s="38">
         <v>31</v>
       </c>
       <c r="C32" s="38"/>
       <c r="D32" s="38"/>
       <c r="E32" s="32"/>
-      <c r="F32" s="34" t="s">
+      <c r="F32" t="s" s="34">
         <v>22</v>
       </c>
       <c r="G32" s="34"/>
       <c r="H32" s="36">
         <f>H31*16%</f>
-        <v>16000</v>
       </c>
       <c r="I32" s="37"/>
       <c r="J32" s="3"/>
@@ -1913,13 +1937,12 @@
       <c r="C33" s="32"/>
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
-      <c r="F33" s="34" t="s">
+      <c r="F33" t="s" s="34">
         <v>23</v>
       </c>
       <c r="G33" s="34"/>
       <c r="H33" s="36">
         <f>H31+H32</f>
-        <v>116000</v>
       </c>
       <c r="I33" s="37"/>
       <c r="J33" s="3"/>

</xml_diff>